<commit_message>
More results and trying db4 filter
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="22">
   <si>
     <t>False Pos</t>
   </si>
@@ -39,12 +39,6 @@
   </si>
   <si>
     <t>Bag of Words</t>
-  </si>
-  <si>
-    <t>Multiresolution Histograms (1st Run - every SVM)</t>
-  </si>
-  <si>
-    <t>Multiresolution Histograms (2nd Run - some SVM)</t>
   </si>
   <si>
     <t>Baseline Multiresolution Histograms</t>
@@ -84,6 +78,18 @@
   </si>
   <si>
     <t>Percentage</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Multiresolution Histograms (1st Run - every SVM, haar)</t>
+  </si>
+  <si>
+    <t>Multiresolution Histograms (2nd Run - some SVM, haar)</t>
+  </si>
+  <si>
+    <t>Multiresolution Histograms (3nd Run - no SVM, bayes NB_THRESH = .5, haar)</t>
   </si>
 </sst>
 </file>
@@ -410,22 +416,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L35"/>
+  <dimension ref="A1:L65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="I57" sqref="I57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C2">
         <v>0.125</v>
@@ -433,43 +439,43 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
         <v>11</v>
       </c>
-      <c r="C6" t="s">
+      <c r="E6" t="s">
         <v>12</v>
       </c>
-      <c r="D6" t="s">
+      <c r="F6" t="s">
         <v>13</v>
       </c>
-      <c r="E6" t="s">
+      <c r="G6" t="s">
         <v>14</v>
       </c>
-      <c r="F6" t="s">
+      <c r="H6" t="s">
         <v>15</v>
       </c>
-      <c r="G6" t="s">
+      <c r="I6" t="s">
         <v>16</v>
       </c>
-      <c r="H6" t="s">
+      <c r="J6" t="s">
         <v>17</v>
-      </c>
-      <c r="I6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J6" t="s">
-        <v>19</v>
       </c>
       <c r="K6" t="s">
         <v>1</v>
@@ -480,7 +486,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -521,7 +527,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -562,7 +568,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -603,7 +609,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -644,7 +650,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -685,7 +691,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -726,7 +732,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -767,7 +773,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -808,7 +814,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B15">
         <f>SUM(B7:B14)/SUM($B$7:$I$14)</f>
@@ -876,7 +882,7 @@
         <v>0.38095238095238093</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="L16">
         <f>(B7+C8+D9+E10+F11+G12+H13+I14) / SUM(B7:I14)</f>
@@ -924,37 +930,37 @@
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" t="s">
         <v>11</v>
       </c>
-      <c r="C21" t="s">
+      <c r="E21" t="s">
         <v>12</v>
       </c>
-      <c r="D21" t="s">
+      <c r="F21" t="s">
         <v>13</v>
       </c>
-      <c r="E21" t="s">
+      <c r="G21" t="s">
         <v>14</v>
       </c>
-      <c r="F21" t="s">
+      <c r="H21" t="s">
         <v>15</v>
       </c>
-      <c r="G21" t="s">
+      <c r="I21" t="s">
         <v>16</v>
       </c>
-      <c r="H21" t="s">
+      <c r="J21" t="s">
         <v>17</v>
-      </c>
-      <c r="I21" t="s">
-        <v>18</v>
-      </c>
-      <c r="J21" t="s">
-        <v>19</v>
       </c>
       <c r="K21" t="s">
         <v>1</v>
@@ -965,7 +971,7 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B22">
         <v>9</v>
@@ -1006,7 +1012,7 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -1047,7 +1053,7 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -1088,7 +1094,7 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B25">
         <v>2</v>
@@ -1129,7 +1135,7 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -1170,7 +1176,7 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -1211,7 +1217,7 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -1252,7 +1258,7 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -1293,7 +1299,7 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B30">
         <f>SUM(B22:B29) / SUM($B$22:$I$29)</f>
@@ -1365,7 +1371,7 @@
         <v>0.375</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="L31">
         <f>(B22+C23+D24+E25+F26+G27+H28+I29) / SUM(B22:I29)</f>
@@ -1409,14 +1415,984 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="1"/>
+      <c r="B36" t="s">
+        <v>9</v>
+      </c>
+      <c r="C36" t="s">
+        <v>10</v>
+      </c>
+      <c r="D36" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36" t="s">
+        <v>12</v>
+      </c>
+      <c r="F36" t="s">
+        <v>13</v>
+      </c>
+      <c r="G36" t="s">
+        <v>14</v>
+      </c>
+      <c r="H36" t="s">
+        <v>15</v>
+      </c>
+      <c r="I36" t="s">
+        <v>16</v>
+      </c>
+      <c r="J36" t="s">
+        <v>17</v>
+      </c>
+      <c r="K36" t="s">
+        <v>1</v>
+      </c>
+      <c r="L36" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>9</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <v>16</v>
+      </c>
+      <c r="G37">
+        <v>1</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="I37">
+        <v>3</v>
+      </c>
+      <c r="J37">
+        <f>SUM(B37:I37)/SUM($B$37:$I$44)</f>
+        <v>0.125</v>
+      </c>
+      <c r="K37">
+        <f>(SUM(B37:I37) - B37) / SUM(B37:I37)</f>
+        <v>1</v>
+      </c>
+      <c r="L37">
+        <f>1-K37</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>10</v>
+      </c>
+      <c r="B38">
+        <v>0</v>
+      </c>
+      <c r="C38">
+        <v>2</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="F38">
+        <v>1</v>
+      </c>
+      <c r="G38">
+        <v>8</v>
+      </c>
+      <c r="H38">
+        <v>4</v>
+      </c>
+      <c r="I38">
+        <v>3</v>
+      </c>
+      <c r="J38">
+        <f t="shared" ref="J38:J44" si="13">SUM(B38:I38)/SUM($B$37:$I$44)</f>
+        <v>0.125</v>
+      </c>
+      <c r="K38">
+        <f>(SUM(B38:I38) - C38) / SUM(B38:I38)</f>
+        <v>0.9</v>
+      </c>
+      <c r="L38">
+        <f t="shared" ref="L38:L44" si="14">1-K38</f>
+        <v>9.9999999999999978E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>11</v>
+      </c>
+      <c r="B39">
+        <v>0</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>14</v>
+      </c>
+      <c r="E39">
+        <v>2</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <v>1</v>
+      </c>
+      <c r="H39">
+        <v>3</v>
+      </c>
+      <c r="I39">
+        <v>0</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="13"/>
+        <v>0.125</v>
+      </c>
+      <c r="K39">
+        <f>(SUM(B39:I39) - D39) / SUM(B39:I39)</f>
+        <v>0.3</v>
+      </c>
+      <c r="L39">
+        <f t="shared" si="14"/>
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>12</v>
+      </c>
+      <c r="B40">
+        <v>0</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="D40">
+        <v>3</v>
+      </c>
+      <c r="E40">
+        <v>10</v>
+      </c>
+      <c r="F40">
+        <v>2</v>
+      </c>
+      <c r="G40">
+        <v>4</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <v>0</v>
+      </c>
+      <c r="J40">
+        <f t="shared" si="13"/>
+        <v>0.125</v>
+      </c>
+      <c r="K40">
+        <f>(SUM(B40:I40) - E40) / SUM(B40:I40)</f>
+        <v>0.5</v>
+      </c>
+      <c r="L40">
+        <f t="shared" si="14"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>13</v>
+      </c>
+      <c r="B41">
+        <v>0</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <v>16</v>
+      </c>
+      <c r="G41">
+        <v>3</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+      <c r="I41">
+        <v>1</v>
+      </c>
+      <c r="J41">
+        <f t="shared" si="13"/>
+        <v>0.125</v>
+      </c>
+      <c r="K41">
+        <f>(SUM(B41:I41) - F41) / SUM(B41:I41)</f>
+        <v>0.2</v>
+      </c>
+      <c r="L41">
+        <f t="shared" si="14"/>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>14</v>
+      </c>
+      <c r="B42">
+        <v>0</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="D42">
+        <v>2</v>
+      </c>
+      <c r="E42">
+        <v>1</v>
+      </c>
+      <c r="F42">
+        <v>11</v>
+      </c>
+      <c r="G42">
+        <v>4</v>
+      </c>
+      <c r="H42">
+        <v>0</v>
+      </c>
+      <c r="I42">
+        <v>1</v>
+      </c>
+      <c r="J42">
+        <f t="shared" si="13"/>
+        <v>0.125</v>
+      </c>
+      <c r="K42">
+        <f>(SUM(B42:I42) - G42) / SUM(B42:I42)</f>
+        <v>0.8</v>
+      </c>
+      <c r="L42">
+        <f t="shared" si="14"/>
+        <v>0.19999999999999996</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>15</v>
+      </c>
+      <c r="B43">
+        <v>0</v>
+      </c>
+      <c r="C43">
+        <v>2</v>
+      </c>
+      <c r="D43">
+        <v>2</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43">
+        <v>2</v>
+      </c>
+      <c r="G43">
+        <v>3</v>
+      </c>
+      <c r="H43">
+        <v>11</v>
+      </c>
+      <c r="I43">
+        <v>0</v>
+      </c>
+      <c r="J43">
+        <f t="shared" si="13"/>
+        <v>0.125</v>
+      </c>
+      <c r="K43">
+        <f>(SUM(B43:I43) - H43) / SUM(B43:I43)</f>
+        <v>0.45</v>
+      </c>
+      <c r="L43">
+        <f t="shared" si="14"/>
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>16</v>
+      </c>
+      <c r="B44">
+        <v>0</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44">
         <v>6</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+      <c r="G44">
+        <v>1</v>
+      </c>
+      <c r="H44">
+        <v>2</v>
+      </c>
+      <c r="I44">
+        <v>10</v>
+      </c>
+      <c r="J44">
+        <f t="shared" si="13"/>
+        <v>0.125</v>
+      </c>
+      <c r="K44">
+        <f>(SUM(B44:I44) - I44) / SUM(B44:I44)</f>
+        <v>0.5</v>
+      </c>
+      <c r="L44">
+        <f t="shared" si="14"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>17</v>
+      </c>
+      <c r="B45">
+        <f>SUM(B37:B44) / SUM($B$37:$I$44)</f>
+        <v>0</v>
+      </c>
+      <c r="C45">
+        <f t="shared" ref="C45:I45" si="15">SUM(C37:C44) / SUM($B$22:$I$29)</f>
+        <v>4.3749999999999997E-2</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="15"/>
+        <v>0.13750000000000001</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="15"/>
+        <v>8.7499999999999994E-2</v>
+      </c>
+      <c r="F45">
+        <f t="shared" si="15"/>
+        <v>0.33750000000000002</v>
+      </c>
+      <c r="G45">
+        <f t="shared" si="15"/>
+        <v>0.15625</v>
+      </c>
+      <c r="H45">
+        <f t="shared" si="15"/>
+        <v>0.125</v>
+      </c>
+      <c r="I45">
+        <f t="shared" si="15"/>
+        <v>0.1125</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>0</v>
+      </c>
+      <c r="C46">
+        <f>(SUM(C37:C44) - C38) / SUM(C37:C44)</f>
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="D46">
+        <f>(SUM(D37:D44) - D39) / SUM(D37:D44)</f>
+        <v>0.36363636363636365</v>
+      </c>
+      <c r="E46">
+        <f>(SUM(E37:E44) - E40) / SUM(E37:E44)</f>
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="F46">
+        <f>(SUM(F37:F44) - F41) / SUM(F37:F44)</f>
+        <v>0.70370370370370372</v>
+      </c>
+      <c r="G46">
+        <f>(SUM(G37:G44) - G42) / SUM(G37:G44)</f>
+        <v>0.84</v>
+      </c>
+      <c r="H46">
+        <f>(SUM(H37:H44) - H43) / SUM(H37:H44)</f>
+        <v>0.45</v>
+      </c>
+      <c r="I46">
+        <f>(SUM(I37:I44) - I44) / SUM(I37:I44)</f>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="K46" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="L46">
+        <f>(B37+C38+D39+E40+F41+G42+H43+I44) / SUM(B37:I44)</f>
+        <v>0.41875000000000001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>3</v>
+      </c>
+      <c r="C47">
+        <f>1-C46</f>
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="D47">
+        <f t="shared" ref="D47:I47" si="16">1-D46</f>
+        <v>0.63636363636363635</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="16"/>
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="16"/>
+        <v>0.29629629629629628</v>
+      </c>
+      <c r="G47">
+        <f t="shared" si="16"/>
+        <v>0.16000000000000003</v>
+      </c>
+      <c r="H47">
+        <f t="shared" si="16"/>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="I47">
+        <f t="shared" si="16"/>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L47">
+        <f>SUM(B37:I44)</f>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B50" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>9</v>
+      </c>
+      <c r="C51" t="s">
+        <v>10</v>
+      </c>
+      <c r="D51" t="s">
+        <v>11</v>
+      </c>
+      <c r="E51" t="s">
+        <v>12</v>
+      </c>
+      <c r="F51" t="s">
+        <v>13</v>
+      </c>
+      <c r="G51" t="s">
+        <v>14</v>
+      </c>
+      <c r="H51" t="s">
+        <v>15</v>
+      </c>
+      <c r="I51" t="s">
+        <v>16</v>
+      </c>
+      <c r="J51" t="s">
+        <v>17</v>
+      </c>
+      <c r="K51" t="s">
+        <v>1</v>
+      </c>
+      <c r="L51" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>9</v>
+      </c>
+      <c r="B52">
+        <v>12</v>
+      </c>
+      <c r="C52">
+        <v>1</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="E52">
+        <v>0</v>
+      </c>
+      <c r="F52">
+        <v>3</v>
+      </c>
+      <c r="G52">
+        <v>1</v>
+      </c>
+      <c r="H52">
+        <v>0</v>
+      </c>
+      <c r="I52">
+        <v>3</v>
+      </c>
+      <c r="J52">
+        <f>SUM(B52:I52)/SUM($B$22:$I$29)</f>
+        <v>0.125</v>
+      </c>
+      <c r="K52">
+        <f>(SUM(B52:I52) - B52) / SUM(B52:I52)</f>
+        <v>0.4</v>
+      </c>
+      <c r="L52">
+        <f>1-K52</f>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>10</v>
+      </c>
+      <c r="B53">
+        <v>1</v>
+      </c>
+      <c r="C53">
+        <v>5</v>
+      </c>
+      <c r="D53">
+        <v>1</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+      <c r="F53">
+        <v>4</v>
+      </c>
+      <c r="G53">
+        <v>1</v>
+      </c>
+      <c r="H53">
+        <v>7</v>
+      </c>
+      <c r="I53">
+        <v>1</v>
+      </c>
+      <c r="J53">
+        <f t="shared" ref="J53:J59" si="17">SUM(B53:I53)/SUM($B$22:$I$29)</f>
+        <v>0.125</v>
+      </c>
+      <c r="K53">
+        <f>(SUM(B53:I53) - C53) / SUM(B53:I53)</f>
+        <v>0.75</v>
+      </c>
+      <c r="L53">
+        <f t="shared" ref="L53:L59" si="18">1-K53</f>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>11</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
+      <c r="D54">
+        <v>14</v>
+      </c>
+      <c r="E54">
+        <v>0</v>
+      </c>
+      <c r="F54">
+        <v>2</v>
+      </c>
+      <c r="G54">
+        <v>0</v>
+      </c>
+      <c r="H54">
+        <v>1</v>
+      </c>
+      <c r="I54">
+        <v>1</v>
+      </c>
+      <c r="J54">
+        <f t="shared" si="17"/>
+        <v>0.125</v>
+      </c>
+      <c r="K54">
+        <f>(SUM(B54:I54) - D54) / SUM(B54:I54)</f>
+        <v>0.3</v>
+      </c>
+      <c r="L54">
+        <f t="shared" si="18"/>
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>12</v>
+      </c>
+      <c r="B55">
+        <v>8</v>
+      </c>
+      <c r="C55">
+        <v>2</v>
+      </c>
+      <c r="D55">
+        <v>3</v>
+      </c>
+      <c r="E55">
+        <v>0</v>
+      </c>
+      <c r="F55">
+        <v>6</v>
+      </c>
+      <c r="G55">
+        <v>0</v>
+      </c>
+      <c r="H55">
+        <v>1</v>
+      </c>
+      <c r="I55">
+        <v>0</v>
+      </c>
+      <c r="J55">
+        <f t="shared" si="17"/>
+        <v>0.125</v>
+      </c>
+      <c r="K55">
+        <f>(SUM(B55:I55) - E55) / SUM(B55:I55)</f>
+        <v>1</v>
+      </c>
+      <c r="L55">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>13</v>
+      </c>
+      <c r="B56">
+        <v>3</v>
+      </c>
+      <c r="C56">
+        <v>2</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
+      <c r="F56">
+        <v>9</v>
+      </c>
+      <c r="G56">
+        <v>1</v>
+      </c>
+      <c r="H56">
+        <v>0</v>
+      </c>
+      <c r="I56">
+        <v>5</v>
+      </c>
+      <c r="J56">
+        <f t="shared" si="17"/>
+        <v>0.125</v>
+      </c>
+      <c r="K56">
+        <f>(SUM(B56:I56) - F56) / SUM(B56:I56)</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="L56">
+        <f t="shared" si="18"/>
+        <v>0.44999999999999996</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>14</v>
+      </c>
+      <c r="B57">
+        <v>4</v>
+      </c>
+      <c r="C57">
+        <v>5</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+      <c r="F57">
+        <v>7</v>
+      </c>
+      <c r="G57">
+        <v>1</v>
+      </c>
+      <c r="H57">
+        <v>0</v>
+      </c>
+      <c r="I57">
+        <v>3</v>
+      </c>
+      <c r="J57">
+        <f t="shared" si="17"/>
+        <v>0.125</v>
+      </c>
+      <c r="K57">
+        <f>(SUM(B57:I57) - G57) / SUM(B57:I57)</f>
+        <v>0.95</v>
+      </c>
+      <c r="L57">
+        <f t="shared" si="18"/>
+        <v>5.0000000000000044E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>15</v>
+      </c>
+      <c r="B58">
+        <v>1</v>
+      </c>
+      <c r="C58">
+        <v>5</v>
+      </c>
+      <c r="D58">
+        <v>2</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
+      <c r="F58">
+        <v>4</v>
+      </c>
+      <c r="G58">
+        <v>0</v>
+      </c>
+      <c r="H58">
+        <v>8</v>
+      </c>
+      <c r="I58">
+        <v>0</v>
+      </c>
+      <c r="J58">
+        <f t="shared" si="17"/>
+        <v>0.125</v>
+      </c>
+      <c r="K58">
+        <f>(SUM(B58:I58) - H58) / SUM(B58:I58)</f>
+        <v>0.6</v>
+      </c>
+      <c r="L58">
+        <f t="shared" si="18"/>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>16</v>
+      </c>
+      <c r="B59">
+        <v>1</v>
+      </c>
+      <c r="C59">
+        <v>8</v>
+      </c>
+      <c r="D59">
+        <v>0</v>
+      </c>
+      <c r="E59">
+        <v>0</v>
+      </c>
+      <c r="F59">
+        <v>4</v>
+      </c>
+      <c r="G59">
+        <v>0</v>
+      </c>
+      <c r="H59">
+        <v>3</v>
+      </c>
+      <c r="I59">
+        <v>4</v>
+      </c>
+      <c r="J59">
+        <f t="shared" si="17"/>
+        <v>0.125</v>
+      </c>
+      <c r="K59">
+        <f>(SUM(B59:I59) - I59) / SUM(B59:I59)</f>
+        <v>0.8</v>
+      </c>
+      <c r="L59">
+        <f t="shared" si="18"/>
+        <v>0.19999999999999996</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>17</v>
+      </c>
+      <c r="B60">
+        <f>SUM(B52:B59) / SUM($B$52:$I$59)</f>
+        <v>0.19375000000000001</v>
+      </c>
+      <c r="C60">
+        <f t="shared" ref="C60:I60" si="19">SUM(C52:C59) / SUM($B$52:$I$59)</f>
+        <v>0.18124999999999999</v>
+      </c>
+      <c r="D60">
+        <f t="shared" si="19"/>
+        <v>0.125</v>
+      </c>
+      <c r="E60">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="F60">
+        <f t="shared" si="19"/>
+        <v>0.24374999999999999</v>
+      </c>
+      <c r="G60">
+        <f t="shared" si="19"/>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="H60">
+        <f t="shared" si="19"/>
+        <v>0.125</v>
+      </c>
+      <c r="I60">
+        <f t="shared" si="19"/>
+        <v>0.10625</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>0</v>
+      </c>
+      <c r="B61">
+        <f>(SUM(B52:B59) - B52) / SUM(B52:B59)</f>
+        <v>0.61290322580645162</v>
+      </c>
+      <c r="C61">
+        <f>(SUM(C52:C59) - C53) / SUM(C52:C59)</f>
+        <v>0.82758620689655171</v>
+      </c>
+      <c r="D61">
+        <f>(SUM(D52:D59) - D54) / SUM(D52:D59)</f>
+        <v>0.3</v>
+      </c>
+      <c r="F61">
+        <f>(SUM(F52:F59) - F56) / SUM(F52:F59)</f>
+        <v>0.76923076923076927</v>
+      </c>
+      <c r="G61">
+        <f>(SUM(G52:G59) - G57) / SUM(G52:G59)</f>
+        <v>0.75</v>
+      </c>
+      <c r="H61">
+        <f>(SUM(H52:H59) - H58) / SUM(H52:H59)</f>
+        <v>0.6</v>
+      </c>
+      <c r="I61">
+        <f>(SUM(I52:I59) - I59) / SUM(I52:I59)</f>
+        <v>0.76470588235294112</v>
+      </c>
+      <c r="K61" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L61">
+        <f>(B52+C53+D54+E55+F56+G57+H58+I59) / SUM(B52:I59)</f>
+        <v>0.33124999999999999</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>3</v>
+      </c>
+      <c r="B62">
+        <f>1-B61</f>
+        <v>0.38709677419354838</v>
+      </c>
+      <c r="C62">
+        <f>1-C61</f>
+        <v>0.17241379310344829</v>
+      </c>
+      <c r="D62">
+        <f t="shared" ref="D62:I62" si="20">1-D61</f>
+        <v>0.7</v>
+      </c>
+      <c r="F62">
+        <f t="shared" si="20"/>
+        <v>0.23076923076923073</v>
+      </c>
+      <c r="G62">
+        <f t="shared" si="20"/>
+        <v>0.25</v>
+      </c>
+      <c r="H62">
+        <f t="shared" si="20"/>
+        <v>0.4</v>
+      </c>
+      <c r="I62">
+        <f t="shared" si="20"/>
+        <v>0.23529411764705888</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated results with db4 run
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="23">
   <si>
     <t>False Pos</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>Multiresolution Histograms (3nd Run - no SVM, bayes NB_THRESH = .5, haar)</t>
+  </si>
+  <si>
+    <t>Multiresolution Histograms (3nd Run - no SVM, bayes NB_THRESH = .5, db4)</t>
   </si>
 </sst>
 </file>
@@ -416,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L65"/>
+  <dimension ref="A1:L79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="I57" sqref="I57"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="E60" sqref="E60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2390,8 +2393,499 @@
         <v>0.23529411764705888</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B65" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>9</v>
+      </c>
+      <c r="C66" t="s">
+        <v>10</v>
+      </c>
+      <c r="D66" t="s">
+        <v>11</v>
+      </c>
+      <c r="E66" t="s">
+        <v>12</v>
+      </c>
+      <c r="F66" t="s">
+        <v>13</v>
+      </c>
+      <c r="G66" t="s">
+        <v>14</v>
+      </c>
+      <c r="H66" t="s">
+        <v>15</v>
+      </c>
+      <c r="I66" t="s">
+        <v>16</v>
+      </c>
+      <c r="J66" t="s">
+        <v>17</v>
+      </c>
+      <c r="K66" t="s">
+        <v>1</v>
+      </c>
+      <c r="L66" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>9</v>
+      </c>
+      <c r="B67">
+        <v>1</v>
+      </c>
+      <c r="C67">
+        <v>0</v>
+      </c>
+      <c r="D67">
+        <v>0</v>
+      </c>
+      <c r="E67">
+        <v>2</v>
+      </c>
+      <c r="F67">
+        <v>13</v>
+      </c>
+      <c r="G67">
+        <v>1</v>
+      </c>
+      <c r="H67">
+        <v>1</v>
+      </c>
+      <c r="I67">
+        <v>2</v>
+      </c>
+      <c r="J67">
+        <f>SUM(B67:I67)/SUM($B$22:$I$29)</f>
+        <v>0.125</v>
+      </c>
+      <c r="K67">
+        <f>(SUM(B67:I67) - B67) / SUM(B67:I67)</f>
+        <v>0.95</v>
+      </c>
+      <c r="L67">
+        <f>1-K67</f>
+        <v>5.0000000000000044E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>10</v>
+      </c>
+      <c r="B68">
+        <v>2</v>
+      </c>
+      <c r="C68">
+        <v>10</v>
+      </c>
+      <c r="D68">
+        <v>0</v>
+      </c>
+      <c r="E68">
+        <v>0</v>
+      </c>
+      <c r="F68">
+        <v>0</v>
+      </c>
+      <c r="G68">
+        <v>3</v>
+      </c>
+      <c r="H68">
+        <v>4</v>
+      </c>
+      <c r="I68">
+        <v>1</v>
+      </c>
+      <c r="J68">
+        <f t="shared" ref="J68:J74" si="21">SUM(B68:I68)/SUM($B$22:$I$29)</f>
+        <v>0.125</v>
+      </c>
+      <c r="K68">
+        <f>(SUM(B68:I68) - C68) / SUM(B68:I68)</f>
+        <v>0.5</v>
+      </c>
+      <c r="L68">
+        <f t="shared" ref="L68:L74" si="22">1-K68</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>11</v>
+      </c>
+      <c r="B69">
+        <v>0</v>
+      </c>
+      <c r="C69">
+        <v>1</v>
+      </c>
+      <c r="D69">
+        <v>15</v>
+      </c>
+      <c r="E69">
+        <v>0</v>
+      </c>
+      <c r="F69">
+        <v>0</v>
+      </c>
+      <c r="G69">
+        <v>0</v>
+      </c>
+      <c r="H69">
+        <v>3</v>
+      </c>
+      <c r="I69">
+        <v>1</v>
+      </c>
+      <c r="J69">
+        <f t="shared" si="21"/>
+        <v>0.125</v>
+      </c>
+      <c r="K69">
+        <f>(SUM(B69:I69) - D69) / SUM(B69:I69)</f>
+        <v>0.25</v>
+      </c>
+      <c r="L69">
+        <f t="shared" si="22"/>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>12</v>
+      </c>
+      <c r="B70">
+        <v>0</v>
+      </c>
+      <c r="C70">
+        <v>8</v>
+      </c>
+      <c r="D70">
+        <v>10</v>
+      </c>
+      <c r="E70">
+        <v>1</v>
+      </c>
+      <c r="F70">
+        <v>0</v>
+      </c>
+      <c r="G70">
+        <v>0</v>
+      </c>
+      <c r="H70">
+        <v>0</v>
+      </c>
+      <c r="I70">
+        <v>1</v>
+      </c>
+      <c r="J70">
+        <f t="shared" si="21"/>
+        <v>0.125</v>
+      </c>
+      <c r="K70">
+        <f>(SUM(B70:I70) - E70) / SUM(B70:I70)</f>
+        <v>0.95</v>
+      </c>
+      <c r="L70">
+        <f t="shared" si="22"/>
+        <v>5.0000000000000044E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>13</v>
+      </c>
+      <c r="B71">
+        <v>0</v>
+      </c>
+      <c r="C71">
+        <v>2</v>
+      </c>
+      <c r="D71">
+        <v>0</v>
+      </c>
+      <c r="E71">
+        <v>1</v>
+      </c>
+      <c r="F71">
+        <v>16</v>
+      </c>
+      <c r="G71">
+        <v>0</v>
+      </c>
+      <c r="H71">
+        <v>1</v>
+      </c>
+      <c r="I71">
+        <v>0</v>
+      </c>
+      <c r="J71">
+        <f t="shared" si="21"/>
+        <v>0.125</v>
+      </c>
+      <c r="K71">
+        <f>(SUM(B71:I71) - F71) / SUM(B71:I71)</f>
+        <v>0.2</v>
+      </c>
+      <c r="L71">
+        <f t="shared" si="22"/>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>14</v>
+      </c>
+      <c r="B72">
+        <v>3</v>
+      </c>
+      <c r="C72">
+        <v>6</v>
+      </c>
+      <c r="D72">
+        <v>3</v>
+      </c>
+      <c r="E72">
+        <v>0</v>
+      </c>
+      <c r="F72">
+        <v>3</v>
+      </c>
+      <c r="G72">
+        <v>2</v>
+      </c>
+      <c r="H72">
+        <v>2</v>
+      </c>
+      <c r="I72">
+        <v>1</v>
+      </c>
+      <c r="J72">
+        <f t="shared" si="21"/>
+        <v>0.125</v>
+      </c>
+      <c r="K72">
+        <f>(SUM(B72:I72) - G72) / SUM(B72:I72)</f>
+        <v>0.9</v>
+      </c>
+      <c r="L72">
+        <f t="shared" si="22"/>
+        <v>9.9999999999999978E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>15</v>
+      </c>
+      <c r="B73">
+        <v>1</v>
+      </c>
+      <c r="C73">
+        <v>4</v>
+      </c>
+      <c r="D73">
+        <v>1</v>
+      </c>
+      <c r="E73">
+        <v>0</v>
+      </c>
+      <c r="F73">
+        <v>0</v>
+      </c>
+      <c r="G73">
+        <v>2</v>
+      </c>
+      <c r="H73">
+        <v>12</v>
+      </c>
+      <c r="I73">
+        <v>0</v>
+      </c>
+      <c r="J73">
+        <f t="shared" si="21"/>
+        <v>0.125</v>
+      </c>
+      <c r="K73">
+        <f>(SUM(B73:I73) - H73) / SUM(B73:I73)</f>
+        <v>0.4</v>
+      </c>
+      <c r="L73">
+        <f t="shared" si="22"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>16</v>
+      </c>
+      <c r="B74">
+        <v>0</v>
+      </c>
+      <c r="C74">
+        <v>2</v>
+      </c>
+      <c r="D74">
+        <v>0</v>
+      </c>
+      <c r="E74">
+        <v>0</v>
+      </c>
+      <c r="F74">
+        <v>6</v>
+      </c>
+      <c r="G74">
+        <v>0</v>
+      </c>
+      <c r="H74">
+        <v>1</v>
+      </c>
+      <c r="I74">
+        <v>11</v>
+      </c>
+      <c r="J74">
+        <f t="shared" si="21"/>
+        <v>0.125</v>
+      </c>
+      <c r="K74">
+        <f>(SUM(B74:I74) - I74) / SUM(B74:I74)</f>
+        <v>0.45</v>
+      </c>
+      <c r="L74">
+        <f t="shared" si="22"/>
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>17</v>
+      </c>
+      <c r="B75">
+        <f>SUM(B67:B74) / SUM($B$52:$I$59)</f>
+        <v>4.3749999999999997E-2</v>
+      </c>
+      <c r="C75">
+        <f t="shared" ref="C75:I75" si="23">SUM(C67:C74) / SUM($B$52:$I$59)</f>
+        <v>0.20624999999999999</v>
+      </c>
+      <c r="D75">
+        <f t="shared" si="23"/>
+        <v>0.18124999999999999</v>
+      </c>
+      <c r="E75">
+        <f t="shared" si="23"/>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="F75">
+        <f t="shared" si="23"/>
+        <v>0.23749999999999999</v>
+      </c>
+      <c r="G75">
+        <f t="shared" si="23"/>
+        <v>0.05</v>
+      </c>
+      <c r="H75">
+        <f t="shared" si="23"/>
+        <v>0.15</v>
+      </c>
+      <c r="I75">
+        <f t="shared" si="23"/>
+        <v>0.10625</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>0</v>
+      </c>
+      <c r="B76">
+        <f>(SUM(B67:B74) - B67) / SUM(B67:B74)</f>
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="C76">
+        <f>(SUM(C67:C74) - C68) / SUM(C67:C74)</f>
+        <v>0.69696969696969702</v>
+      </c>
+      <c r="D76">
+        <f>(SUM(D67:D74) - D69) / SUM(D67:D74)</f>
+        <v>0.48275862068965519</v>
+      </c>
+      <c r="E76">
+        <f>(SUM(E67:E74) - E69) / SUM(E67:E74)</f>
+        <v>1</v>
+      </c>
+      <c r="F76">
+        <f>(SUM(F67:F74) - F71) / SUM(F67:F74)</f>
+        <v>0.57894736842105265</v>
+      </c>
+      <c r="G76">
+        <f>(SUM(G67:G74) - G72) / SUM(G67:G74)</f>
+        <v>0.75</v>
+      </c>
+      <c r="H76">
+        <f>(SUM(H67:H74) - H73) / SUM(H67:H74)</f>
+        <v>0.5</v>
+      </c>
+      <c r="I76">
+        <f>(SUM(I67:I74) - I74) / SUM(I67:I74)</f>
+        <v>0.35294117647058826</v>
+      </c>
+      <c r="K76" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L76">
+        <f>(B67+C68+D69+E70+F71+G72+H73+I74) / SUM(B67:I74)</f>
+        <v>0.42499999999999999</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>3</v>
+      </c>
+      <c r="B77">
+        <f>1-B76</f>
+        <v>0.1428571428571429</v>
+      </c>
+      <c r="C77">
+        <f>1-C76</f>
+        <v>0.30303030303030298</v>
+      </c>
+      <c r="D77">
+        <f t="shared" ref="D77:I77" si="24">1-D76</f>
+        <v>0.51724137931034475</v>
+      </c>
+      <c r="E77">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="F77">
+        <f t="shared" ref="F77:I77" si="25">1-F76</f>
+        <v>0.42105263157894735</v>
+      </c>
+      <c r="G77">
+        <f t="shared" si="25"/>
+        <v>0.25</v>
+      </c>
+      <c r="H77">
+        <f t="shared" si="25"/>
+        <v>0.5</v>
+      </c>
+      <c r="I77">
+        <f t="shared" si="25"/>
+        <v>0.64705882352941169</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Posted results from baseline
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="23">
   <si>
     <t>False Pos</t>
   </si>
@@ -419,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L79"/>
+  <dimension ref="A1:L90"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+      <selection activeCell="M80" sqref="M80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2889,6 +2889,330 @@
         <v>5</v>
       </c>
     </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J80" t="s">
+        <v>17</v>
+      </c>
+      <c r="K80" t="s">
+        <v>1</v>
+      </c>
+      <c r="L80" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B81">
+        <v>0</v>
+      </c>
+      <c r="C81">
+        <v>1</v>
+      </c>
+      <c r="D81">
+        <v>0</v>
+      </c>
+      <c r="E81">
+        <v>0</v>
+      </c>
+      <c r="F81">
+        <v>18</v>
+      </c>
+      <c r="G81">
+        <v>0</v>
+      </c>
+      <c r="H81">
+        <v>0</v>
+      </c>
+      <c r="I81">
+        <v>1</v>
+      </c>
+      <c r="J81">
+        <f>SUM(B81:I81)/SUM($B$22:$I$29)</f>
+        <v>0.125</v>
+      </c>
+      <c r="K81">
+        <f>(SUM(B81:I81) - B81) / SUM(B81:I81)</f>
+        <v>1</v>
+      </c>
+      <c r="L81">
+        <f>1-K81</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B82">
+        <v>0</v>
+      </c>
+      <c r="C82">
+        <v>12</v>
+      </c>
+      <c r="D82">
+        <v>2</v>
+      </c>
+      <c r="E82">
+        <v>1</v>
+      </c>
+      <c r="F82">
+        <v>1</v>
+      </c>
+      <c r="G82">
+        <v>1</v>
+      </c>
+      <c r="H82">
+        <v>2</v>
+      </c>
+      <c r="I82">
+        <v>1</v>
+      </c>
+      <c r="J82">
+        <f t="shared" ref="J82:J88" si="26">SUM(B82:I82)/SUM($B$22:$I$29)</f>
+        <v>0.125</v>
+      </c>
+      <c r="K82">
+        <f>(SUM(B82:I82) - C82) / SUM(B82:I82)</f>
+        <v>0.4</v>
+      </c>
+      <c r="L82">
+        <f t="shared" ref="L82:L88" si="27">1-K82</f>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="83" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B83">
+        <v>0</v>
+      </c>
+      <c r="C83">
+        <v>0</v>
+      </c>
+      <c r="D83">
+        <v>17</v>
+      </c>
+      <c r="E83">
+        <v>0</v>
+      </c>
+      <c r="F83">
+        <v>0</v>
+      </c>
+      <c r="G83">
+        <v>0</v>
+      </c>
+      <c r="H83">
+        <v>3</v>
+      </c>
+      <c r="I83">
+        <v>0</v>
+      </c>
+      <c r="J83">
+        <f t="shared" si="26"/>
+        <v>0.125</v>
+      </c>
+      <c r="K83">
+        <f>(SUM(B83:I83) - D83) / SUM(B83:I83)</f>
+        <v>0.15</v>
+      </c>
+      <c r="L83">
+        <f t="shared" si="27"/>
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="84" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B84">
+        <v>0</v>
+      </c>
+      <c r="C84">
+        <v>4</v>
+      </c>
+      <c r="D84">
+        <v>11</v>
+      </c>
+      <c r="E84">
+        <v>2</v>
+      </c>
+      <c r="F84">
+        <v>0</v>
+      </c>
+      <c r="G84">
+        <v>2</v>
+      </c>
+      <c r="H84">
+        <v>1</v>
+      </c>
+      <c r="I84">
+        <v>0</v>
+      </c>
+      <c r="J84">
+        <f t="shared" si="26"/>
+        <v>0.125</v>
+      </c>
+      <c r="K84">
+        <f>(SUM(B84:I84) - E84) / SUM(B84:I84)</f>
+        <v>0.9</v>
+      </c>
+      <c r="L84">
+        <f t="shared" si="27"/>
+        <v>9.9999999999999978E-2</v>
+      </c>
+    </row>
+    <row r="85" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B85">
+        <v>0</v>
+      </c>
+      <c r="C85">
+        <v>1</v>
+      </c>
+      <c r="D85">
+        <v>0</v>
+      </c>
+      <c r="E85">
+        <v>0</v>
+      </c>
+      <c r="F85">
+        <v>19</v>
+      </c>
+      <c r="G85">
+        <v>0</v>
+      </c>
+      <c r="H85">
+        <v>0</v>
+      </c>
+      <c r="I85">
+        <v>0</v>
+      </c>
+      <c r="J85">
+        <f t="shared" si="26"/>
+        <v>0.125</v>
+      </c>
+      <c r="K85">
+        <f>(SUM(B85:I85) - F85) / SUM(B85:I85)</f>
+        <v>0.05</v>
+      </c>
+      <c r="L85">
+        <f t="shared" si="27"/>
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="86" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B86">
+        <v>0</v>
+      </c>
+      <c r="C86">
+        <v>7</v>
+      </c>
+      <c r="D86">
+        <v>3</v>
+      </c>
+      <c r="E86">
+        <v>0</v>
+      </c>
+      <c r="F86">
+        <v>9</v>
+      </c>
+      <c r="G86">
+        <v>0</v>
+      </c>
+      <c r="H86">
+        <v>0</v>
+      </c>
+      <c r="I86">
+        <v>1</v>
+      </c>
+      <c r="J86">
+        <f t="shared" si="26"/>
+        <v>0.125</v>
+      </c>
+      <c r="K86">
+        <f>(SUM(B86:I86) - G86) / SUM(B86:I86)</f>
+        <v>1</v>
+      </c>
+      <c r="L86">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B87">
+        <v>0</v>
+      </c>
+      <c r="C87">
+        <v>3</v>
+      </c>
+      <c r="D87">
+        <v>2</v>
+      </c>
+      <c r="E87">
+        <v>0</v>
+      </c>
+      <c r="F87">
+        <v>0</v>
+      </c>
+      <c r="G87">
+        <v>0</v>
+      </c>
+      <c r="H87">
+        <v>15</v>
+      </c>
+      <c r="I87">
+        <v>0</v>
+      </c>
+      <c r="J87">
+        <f t="shared" si="26"/>
+        <v>0.125</v>
+      </c>
+      <c r="K87">
+        <f>(SUM(B87:I87) - H87) / SUM(B87:I87)</f>
+        <v>0.25</v>
+      </c>
+      <c r="L87">
+        <f t="shared" si="27"/>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="88" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B88">
+        <v>0</v>
+      </c>
+      <c r="C88">
+        <v>4</v>
+      </c>
+      <c r="D88">
+        <v>0</v>
+      </c>
+      <c r="E88">
+        <v>0</v>
+      </c>
+      <c r="F88">
+        <v>4</v>
+      </c>
+      <c r="G88">
+        <v>0</v>
+      </c>
+      <c r="H88">
+        <v>3</v>
+      </c>
+      <c r="I88">
+        <v>9</v>
+      </c>
+      <c r="J88">
+        <f t="shared" si="26"/>
+        <v>0.125</v>
+      </c>
+      <c r="K88">
+        <f>(SUM(B88:I88) - I88) / SUM(B88:I88)</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="L88">
+        <f t="shared" si="27"/>
+        <v>0.44999999999999996</v>
+      </c>
+    </row>
+    <row r="90" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="K90" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L90">
+        <f>(B81+C82+D83+E84+F85+G86+H87+I88) / SUM(B81:I88)</f>
+        <v>0.46250000000000002</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>